<commit_message>
Version de vista de piezas 2D agregada
</commit_message>
<xml_diff>
--- a/Records/Test1.xlsx
+++ b/Records/Test1.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -458,6 +458,60 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AG-RH-LW-UP</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Derecho</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SPUFLW-LH </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Izquierdo</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>